<commit_message>
增加了local view, global view, single, sequential
</commit_message>
<xml_diff>
--- a/test/content.xlsx
+++ b/test/content.xlsx
@@ -1979,7 +1979,7 @@
       </c>
       <c r="E52" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2909,7 +2909,7 @@
       </c>
       <c r="E114" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="19.5">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3449,7 +3449,7 @@
       </c>
       <c r="E150" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="19.5">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -4124,7 +4124,7 @@
       </c>
       <c r="E195" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="19.5">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -4439,7 +4439,7 @@
       </c>
       <c r="E216" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="19.5">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -4604,7 +4604,7 @@
       </c>
       <c r="E227" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="19.5">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="E243" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="244" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="244" customHeight="1" ht="19.5">
       <c r="A244" s="1">
         <v>242</v>
       </c>

</xml_diff>